<commit_message>
Actualización datos y corrección formato CSV argentino
- Modificado normalizer para leer formato argentino (punto como separador de miles)
- Agregada página 3: Rangos por Jerarquía (recuperada desde GitHub)
- Actualizados datos procesados con nuevo CSV
- Estadísticas recalculadas con datos reales (sin modificaciones manuales)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/processed/estadisticas_salarios.xlsx
+++ b/data/processed/estadisticas_salarios.xlsx
@@ -505,859 +505,861 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ceo</t>
+          <t>Jefe Admin Conta</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>340</v>
+        <v>43</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2600000</v>
       </c>
       <c r="D2" t="n">
-        <v>4108550</v>
+        <v>2900000</v>
       </c>
       <c r="E2" t="n">
-        <v>8697500</v>
+        <v>3261187.5</v>
       </c>
       <c r="F2" t="n">
-        <v>5815614.132352941</v>
+        <v>3026340.651162791</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>2735000</v>
       </c>
       <c r="H2" t="n">
-        <v>6250000</v>
+        <v>3138000</v>
       </c>
       <c r="I2" t="n">
-        <v>11635500</v>
+        <v>3910000</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>2355996</v>
       </c>
       <c r="K2" t="n">
-        <v>3256024</v>
+        <v>2848000</v>
       </c>
       <c r="L2" t="n">
-        <v>7200000</v>
+        <v>3138000</v>
       </c>
       <c r="M2" t="n">
-        <v>91.95190207443189</v>
+        <v>10.18258426966292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ceo.1</t>
+          <t>Analista Contabilidad</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>340</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1540000</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1680000</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1949999</v>
       </c>
       <c r="F3" t="n">
-        <v>253985.1764705882</v>
+        <v>1791032.43902439</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1577800</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1800000</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1940999.25</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1538760.5</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1680000</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr"/>
+        <v>2045704</v>
+      </c>
+      <c r="M3" t="n">
+        <v>7.142857142857142</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jefe Admin Conta</t>
+          <t>Empleado Administrativo</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>230</v>
+        <v>35</v>
       </c>
       <c r="C4" t="n">
-        <v>2600000</v>
+        <v>1164255</v>
       </c>
       <c r="D4" t="n">
-        <v>2896210.5</v>
+        <v>1270000</v>
       </c>
       <c r="E4" t="n">
-        <v>3270000</v>
+        <v>1400000</v>
       </c>
       <c r="F4" t="n">
-        <v>3327883.652173913</v>
+        <v>1308876.714285714</v>
       </c>
       <c r="G4" t="n">
-        <v>2600000</v>
+        <v>1227500</v>
       </c>
       <c r="H4" t="n">
-        <v>3000000</v>
+        <v>1296070</v>
       </c>
       <c r="I4" t="n">
-        <v>3640000</v>
+        <v>1325000</v>
       </c>
       <c r="J4" t="n">
-        <v>2355500</v>
+        <v>1164255</v>
       </c>
       <c r="K4" t="n">
-        <v>2848000</v>
+        <v>1270000</v>
       </c>
       <c r="L4" t="n">
-        <v>3154967</v>
+        <v>1407150</v>
       </c>
       <c r="M4" t="n">
-        <v>5.337078651685393</v>
+        <v>2.052755905511811</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Analista Contabilidad</t>
+          <t>Analista Cuentas Pagar</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>215</v>
+        <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>1500000</v>
+        <v>1404273.75</v>
       </c>
       <c r="D5" t="n">
-        <v>1680000</v>
+        <v>1600000</v>
       </c>
       <c r="E5" t="n">
-        <v>1991408</v>
+        <v>1714250</v>
       </c>
       <c r="F5" t="n">
-        <v>1787816.023255814</v>
+        <v>1596667.411764706</v>
       </c>
       <c r="G5" t="n">
-        <v>1500000</v>
+        <v>1476700</v>
       </c>
       <c r="H5" t="n">
-        <v>1622000</v>
+        <v>1600000</v>
       </c>
       <c r="I5" t="n">
-        <v>1932670</v>
+        <v>1720000</v>
       </c>
       <c r="J5" t="n">
-        <v>1558140.75</v>
+        <v>1385000</v>
       </c>
       <c r="K5" t="n">
-        <v>1685000</v>
+        <v>1600500</v>
       </c>
       <c r="L5" t="n">
-        <v>2100000</v>
+        <v>1816506.5</v>
       </c>
       <c r="M5" t="n">
-        <v>-3.738872403560831</v>
+        <v>-0.03124023742580443</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Gerente Admin Conta</t>
+          <t>Jefe Produccion</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>185</v>
+        <v>33</v>
       </c>
       <c r="C6" t="n">
-        <v>3600000</v>
+        <v>2441880</v>
       </c>
       <c r="D6" t="n">
-        <v>4500000</v>
+        <v>2850000</v>
       </c>
       <c r="E6" t="n">
-        <v>6246732</v>
+        <v>3400000</v>
       </c>
       <c r="F6" t="n">
-        <v>5134831.648648649</v>
+        <v>3088920.181818182</v>
       </c>
       <c r="G6" t="n">
-        <v>3600000</v>
+        <v>2900000</v>
       </c>
       <c r="H6" t="n">
-        <v>5117500</v>
+        <v>3300000</v>
       </c>
       <c r="I6" t="n">
-        <v>6922214</v>
+        <v>3900000</v>
       </c>
       <c r="J6" t="n">
-        <v>3132530</v>
+        <v>2241741.5</v>
       </c>
       <c r="K6" t="n">
-        <v>4500000</v>
+        <v>2803973</v>
       </c>
       <c r="L6" t="n">
-        <v>6246732</v>
+        <v>3316000</v>
       </c>
       <c r="M6" t="n">
-        <v>13.72222222222222</v>
+        <v>17.69014894223304</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Analista Cuentas Pagar</t>
+          <t>Ejecutivo Ventas</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>32</v>
       </c>
       <c r="C7" t="n">
-        <v>1380000</v>
+        <v>1638520</v>
       </c>
       <c r="D7" t="n">
+        <v>1992720.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3025000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2392020.78125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1850000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2200000</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3100000</v>
+      </c>
+      <c r="J7" t="n">
         <v>1600000</v>
       </c>
-      <c r="E7" t="n">
-        <v>1720000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1552191.2</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1476700</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1506899</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1628000</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1380000</v>
-      </c>
       <c r="K7" t="n">
-        <v>1600500</v>
+        <v>1894257.5</v>
       </c>
       <c r="L7" t="n">
-        <v>1856342</v>
+        <v>3025000</v>
       </c>
       <c r="M7" t="n">
-        <v>-5.848234926585442</v>
+        <v>16.14049304278853</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Empleado Administrativo</t>
+          <t>Gerente Admin Conta</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>175</v>
+        <v>31</v>
       </c>
       <c r="C8" t="n">
-        <v>1154000</v>
+        <v>4191113.5</v>
       </c>
       <c r="D8" t="n">
-        <v>1270000</v>
+        <v>4760326</v>
       </c>
       <c r="E8" t="n">
-        <v>1400000</v>
+        <v>6711107</v>
       </c>
       <c r="F8" t="n">
-        <v>1308876.714285714</v>
+        <v>5729025.870967742</v>
       </c>
       <c r="G8" t="n">
-        <v>1165286</v>
+        <v>4440000</v>
       </c>
       <c r="H8" t="n">
-        <v>1281070</v>
+        <v>5235000</v>
       </c>
       <c r="I8" t="n">
-        <v>1325000</v>
+        <v>6922214</v>
       </c>
       <c r="J8" t="n">
-        <v>1154000</v>
+        <v>4075000</v>
       </c>
       <c r="K8" t="n">
-        <v>1270000</v>
+        <v>4522050</v>
       </c>
       <c r="L8" t="n">
-        <v>1414300</v>
+        <v>6310049</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8716535433070867</v>
+        <v>15.76607954356984</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ejecutivo Ventas</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>175</v>
+        <v>31</v>
       </c>
       <c r="C9" t="n">
+        <v>1546090</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1652000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1921889.580645161</v>
+      </c>
+      <c r="G9" t="n">
         <v>1600000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="H9" t="n">
+        <v>1692000</v>
+      </c>
+      <c r="I9" t="n">
         <v>1900000</v>
       </c>
-      <c r="E9" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="F9" t="n">
-        <v>2317876.142857143</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1622000</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2050000</v>
-      </c>
-      <c r="I9" t="n">
-        <v>3000000</v>
-      </c>
       <c r="J9" t="n">
-        <v>1600000</v>
+        <v>1544135</v>
       </c>
       <c r="K9" t="n">
-        <v>1807229</v>
+        <v>1641285</v>
       </c>
       <c r="L9" t="n">
-        <v>3000000</v>
+        <v>1975000</v>
       </c>
       <c r="M9" t="n">
-        <v>13.43332803977803</v>
+        <v>3.089956954459463</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jefe Produccion</t>
+          <t>Analista Facturacion</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>165</v>
+        <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>2441880</v>
+        <v>1367990.5</v>
       </c>
       <c r="D10" t="n">
-        <v>2850000</v>
+        <v>1500000</v>
       </c>
       <c r="E10" t="n">
-        <v>3400000</v>
+        <v>1656000</v>
       </c>
       <c r="F10" t="n">
-        <v>3088920.181818182</v>
+        <v>1514282.518518518</v>
       </c>
       <c r="G10" t="n">
-        <v>2600000</v>
+        <v>1391294.5</v>
       </c>
       <c r="H10" t="n">
-        <v>3300000</v>
+        <v>1490000</v>
       </c>
       <c r="I10" t="n">
-        <v>3800000</v>
+        <v>1605000</v>
       </c>
       <c r="J10" t="n">
-        <v>2179102</v>
+        <v>1331847</v>
       </c>
       <c r="K10" t="n">
-        <v>2803973</v>
+        <v>1400000</v>
       </c>
       <c r="L10" t="n">
-        <v>3380000</v>
+        <v>1645500</v>
       </c>
       <c r="M10" t="n">
-        <v>17.69014894223304</v>
+        <v>6.428571428571428</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Ceo</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>160</v>
+        <v>26</v>
       </c>
       <c r="C11" t="n">
-        <v>1548045</v>
+        <v>7227500</v>
       </c>
       <c r="D11" t="n">
-        <v>1672000</v>
+        <v>10080000</v>
       </c>
       <c r="E11" t="n">
-        <v>2025000</v>
+        <v>12750000</v>
       </c>
       <c r="F11" t="n">
-        <v>2436894.59375</v>
+        <v>12526837.23076923</v>
       </c>
       <c r="G11" t="n">
-        <v>1564000</v>
+        <v>10678875</v>
       </c>
       <c r="H11" t="n">
-        <v>1756750</v>
+        <v>15817750</v>
       </c>
       <c r="I11" t="n">
-        <v>2693000</v>
+        <v>26722374.5</v>
       </c>
       <c r="J11" t="n">
-        <v>1542180</v>
+        <v>6875000</v>
       </c>
       <c r="K11" t="n">
-        <v>1641285</v>
+        <v>8630000</v>
       </c>
       <c r="L11" t="n">
-        <v>2000000</v>
+        <v>11569500</v>
       </c>
       <c r="M11" t="n">
-        <v>7.035036571954293</v>
+        <v>83.28794901506373</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Analista Facturacion</t>
+          <t>Jefe Rrhh</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="C12" t="n">
-        <v>1378916</v>
+        <v>2146466</v>
       </c>
       <c r="D12" t="n">
-        <v>1560065</v>
+        <v>2580000</v>
       </c>
       <c r="E12" t="n">
-        <v>1800000</v>
+        <v>3000000</v>
       </c>
       <c r="F12" t="n">
-        <v>1651319.555555556</v>
+        <v>2930120</v>
       </c>
       <c r="G12" t="n">
-        <v>1495000</v>
+        <v>2437238</v>
       </c>
       <c r="H12" t="n">
-        <v>1550032.5</v>
+        <v>2580000</v>
       </c>
       <c r="I12" t="n">
-        <v>1773600</v>
+        <v>3000000</v>
       </c>
       <c r="J12" t="n">
-        <v>1350000</v>
+        <v>2031332</v>
       </c>
       <c r="K12" t="n">
-        <v>1566265</v>
+        <v>2287700</v>
       </c>
       <c r="L12" t="n">
-        <v>1870000</v>
+        <v>2750000</v>
       </c>
       <c r="M12" t="n">
-        <v>-1.036382732168567</v>
+        <v>12.77702495956638</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jefe Ventas</t>
+          <t>Analista Admin Personal</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="C13" t="n">
-        <v>2300000</v>
+        <v>1475000</v>
       </c>
       <c r="D13" t="n">
-        <v>2742000</v>
+        <v>1573407</v>
       </c>
       <c r="E13" t="n">
-        <v>3823370</v>
+        <v>1800000</v>
       </c>
       <c r="F13" t="n">
-        <v>3141387.423076923</v>
+        <v>1610904.52173913</v>
       </c>
       <c r="G13" t="n">
-        <v>2391125</v>
+        <v>1551750</v>
       </c>
       <c r="H13" t="n">
-        <v>2955012</v>
+        <v>1636703.5</v>
       </c>
       <c r="I13" t="n">
-        <v>4650150</v>
+        <v>1800000</v>
       </c>
       <c r="J13" t="n">
-        <v>2300000</v>
+        <v>1350000</v>
       </c>
       <c r="K13" t="n">
-        <v>2457626.5</v>
+        <v>1570354</v>
       </c>
       <c r="L13" t="n">
-        <v>3525470</v>
+        <v>1624489</v>
       </c>
       <c r="M13" t="n">
-        <v>20.23844957726489</v>
+        <v>4.225130129894278</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Gerente Planta</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="C14" t="n">
-        <v>2367000</v>
+        <v>4157500</v>
       </c>
       <c r="D14" t="n">
-        <v>2825000</v>
+        <v>5000000</v>
       </c>
       <c r="E14" t="n">
-        <v>3560000</v>
+        <v>6740732.5</v>
       </c>
       <c r="F14" t="n">
-        <v>2972496.84</v>
+        <v>5967663.478260869</v>
       </c>
       <c r="G14" t="n">
-        <v>2254500</v>
+        <v>4798750</v>
       </c>
       <c r="H14" t="n">
-        <v>2500000</v>
+        <v>7000000</v>
       </c>
       <c r="I14" t="n">
-        <v>2933750</v>
+        <v>11296747</v>
       </c>
       <c r="J14" t="n">
-        <v>2785028</v>
+        <v>3523651.25</v>
       </c>
       <c r="K14" t="n">
-        <v>3030660</v>
+        <v>4595827.5</v>
       </c>
       <c r="L14" t="n">
-        <v>3731325</v>
+        <v>5744937.5</v>
       </c>
       <c r="M14" t="n">
-        <v>-17.50971735529555</v>
+        <v>52.31207002438624</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jefe Rrhh</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>2146466</v>
+        <v>2767514</v>
       </c>
       <c r="D15" t="n">
-        <v>2580000</v>
+        <v>3030660</v>
       </c>
       <c r="E15" t="n">
-        <v>3000000</v>
+        <v>3638705.5</v>
       </c>
       <c r="F15" t="n">
-        <v>2930120</v>
+        <v>3194667.652173913</v>
       </c>
       <c r="G15" t="n">
-        <v>2446809.5</v>
+        <v>2750000</v>
       </c>
       <c r="H15" t="n">
-        <v>2600000</v>
+        <v>3260000</v>
       </c>
       <c r="I15" t="n">
-        <v>3350138.75</v>
+        <v>3500000</v>
       </c>
       <c r="J15" t="n">
-        <v>2031332</v>
+        <v>2576014</v>
       </c>
       <c r="K15" t="n">
-        <v>2287700</v>
+        <v>3020918</v>
       </c>
       <c r="L15" t="n">
-        <v>2750000</v>
+        <v>3580000</v>
       </c>
       <c r="M15" t="n">
-        <v>13.65126546312891</v>
+        <v>7.914216804295912</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Gerente Planta</t>
+          <t>Analista Cobranzas</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C16" t="n">
-        <v>3882883.75</v>
+        <v>1353796.25</v>
       </c>
       <c r="D16" t="n">
-        <v>4850000</v>
+        <v>1514050</v>
       </c>
       <c r="E16" t="n">
-        <v>6632348.75</v>
+        <v>1798506.5</v>
       </c>
       <c r="F16" t="n">
-        <v>5674844.166666667</v>
+        <v>1580097.318181818</v>
       </c>
       <c r="G16" t="n">
-        <v>4481250</v>
+        <v>1385000</v>
       </c>
       <c r="H16" t="n">
-        <v>5227500</v>
+        <v>1600000</v>
       </c>
       <c r="I16" t="n">
-        <v>7167973.75</v>
+        <v>1616500</v>
       </c>
       <c r="J16" t="n">
-        <v>3523651.25</v>
+        <v>1348532</v>
       </c>
       <c r="K16" t="n">
-        <v>4595827.5</v>
+        <v>1464434</v>
       </c>
       <c r="L16" t="n">
-        <v>5744937.5</v>
+        <v>1870000</v>
       </c>
       <c r="M16" t="n">
-        <v>13.74447800749702</v>
+        <v>9.25722838994451</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Gerente Ventas</t>
+          <t>Analista Logistica</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C17" t="n">
-        <v>3850000</v>
+        <v>1300000</v>
       </c>
       <c r="D17" t="n">
-        <v>5122000</v>
+        <v>1600000</v>
       </c>
       <c r="E17" t="n">
-        <v>6922214</v>
+        <v>1900000</v>
       </c>
       <c r="F17" t="n">
-        <v>5946885.869565218</v>
+        <v>1762187.285714286</v>
       </c>
       <c r="G17" t="n">
-        <v>3820000</v>
+        <v>1300000</v>
       </c>
       <c r="H17" t="n">
-        <v>5257000</v>
+        <v>1573400</v>
       </c>
       <c r="I17" t="n">
-        <v>6922214</v>
+        <v>1600000</v>
       </c>
       <c r="J17" t="n">
-        <v>3962500</v>
+        <v>1407687.5</v>
       </c>
       <c r="K17" t="n">
-        <v>4664239</v>
+        <v>1680392</v>
       </c>
       <c r="L17" t="n">
-        <v>6395786.75</v>
+        <v>1875000</v>
       </c>
       <c r="M17" t="n">
-        <v>12.70863264082308</v>
+        <v>-6.367085775223877</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Analista Admin Personal</t>
+          <t>Responsable Liquidacion</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C18" t="n">
-        <v>1450000</v>
+        <v>1863500</v>
       </c>
       <c r="D18" t="n">
-        <v>1573407</v>
+        <v>2200000</v>
       </c>
       <c r="E18" t="n">
-        <v>1800000</v>
+        <v>2614457</v>
       </c>
       <c r="F18" t="n">
-        <v>1610904.52173913</v>
+        <v>2362442.666666667</v>
       </c>
       <c r="G18" t="n">
-        <v>1522500</v>
+        <v>2062500</v>
       </c>
       <c r="H18" t="n">
-        <v>1636703.5</v>
+        <v>2200000</v>
       </c>
       <c r="I18" t="n">
-        <v>1800000</v>
+        <v>2693750</v>
       </c>
       <c r="J18" t="n">
-        <v>1250000</v>
+        <v>1741602</v>
       </c>
       <c r="K18" t="n">
-        <v>1570354</v>
+        <v>2002305</v>
       </c>
       <c r="L18" t="n">
-        <v>1628978</v>
+        <v>2270000</v>
       </c>
       <c r="M18" t="n">
-        <v>4.225130129894278</v>
+        <v>9.873370939991661</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Director Comercial</t>
+          <t>Jefe Ventas</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="C19" t="n">
-        <v>4432300</v>
+        <v>2519750</v>
       </c>
       <c r="D19" t="n">
-        <v>5700000</v>
+        <v>3225022.5</v>
       </c>
       <c r="E19" t="n">
-        <v>10769000</v>
+        <v>4300050</v>
       </c>
       <c r="F19" t="n">
-        <v>7956053.681818182</v>
+        <v>3578490.85</v>
       </c>
       <c r="G19" t="n">
-        <v>5442500</v>
+        <v>2900000</v>
       </c>
       <c r="H19" t="n">
-        <v>12500000</v>
+        <v>4200000</v>
       </c>
       <c r="I19" t="n">
-        <v>16070936.75</v>
+        <v>5000000</v>
       </c>
       <c r="J19" t="n">
-        <v>3488000</v>
+        <v>2336126.5</v>
       </c>
       <c r="K19" t="n">
-        <v>5254850</v>
+        <v>2684000</v>
       </c>
       <c r="L19" t="n">
-        <v>9381000</v>
+        <v>3662735</v>
       </c>
       <c r="M19" t="n">
-        <v>137.8754864553698</v>
+        <v>56.48286140089419</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Analista Logistica</t>
+          <t>Gerente Rrhh</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>1300000</v>
+        <v>3350311.5</v>
       </c>
       <c r="D20" t="n">
-        <v>1588756</v>
+        <v>4823000</v>
       </c>
       <c r="E20" t="n">
-        <v>1900000</v>
+        <v>6887500</v>
       </c>
       <c r="F20" t="n">
-        <v>1721860.590909091</v>
+        <v>5234530.1</v>
       </c>
       <c r="G20" t="n">
-        <v>1168750</v>
+        <v>4200000</v>
       </c>
       <c r="H20" t="n">
-        <v>1436700</v>
+        <v>4300126</v>
       </c>
       <c r="I20" t="n">
-        <v>1719276.75</v>
+        <v>7700000</v>
       </c>
       <c r="J20" t="n">
-        <v>1400000</v>
+        <v>3127500</v>
       </c>
       <c r="K20" t="n">
-        <v>1680392</v>
+        <v>4061100</v>
       </c>
       <c r="L20" t="n">
-        <v>1900000</v>
+        <v>6019573.5</v>
       </c>
       <c r="M20" t="n">
-        <v>-14.50209236892344</v>
+        <v>5.885745241437049</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Analista Cobranzas</t>
+          <t>Jefe Logistica</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>1348532</v>
+        <v>2296597.5</v>
       </c>
       <c r="D21" t="n">
-        <v>1514050</v>
+        <v>2840897.5</v>
       </c>
       <c r="E21" t="n">
-        <v>1856342</v>
+        <v>3320583.5</v>
       </c>
       <c r="F21" t="n">
-        <v>1580097.318181818</v>
+        <v>3067139.45</v>
       </c>
       <c r="G21" t="n">
-        <v>1470000</v>
+        <v>2200000</v>
       </c>
       <c r="H21" t="n">
-        <v>1600000</v>
+        <v>2500000</v>
       </c>
       <c r="I21" t="n">
-        <v>1623404</v>
+        <v>3000000</v>
       </c>
       <c r="J21" t="n">
-        <v>1348532</v>
+        <v>2500000</v>
       </c>
       <c r="K21" t="n">
-        <v>1464434</v>
+        <v>2866795</v>
       </c>
       <c r="L21" t="n">
-        <v>1870000</v>
+        <v>3552281</v>
       </c>
       <c r="M21" t="n">
-        <v>9.25722838994451</v>
+        <v>-12.79460163701974</v>
       </c>
     </row>
   </sheetData>
@@ -1399,451 +1401,451 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>salario_ceo</t>
+          <t>salario_jefe_admin_conta</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ceo</t>
+          <t>Jefe Admin Conta</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>340</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>salario_ceo.1</t>
+          <t>salario_analista_contabilidad</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ceo.1</t>
+          <t>Analista Contabilidad</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>340</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>salario_jefe_admin_conta</t>
+          <t>salario_empleado_administrativo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jefe Admin Conta</t>
+          <t>Empleado Administrativo</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>230</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>salario_analista_contabilidad</t>
+          <t>salario_analista_cuentas_pagar</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Analista Contabilidad</t>
+          <t>Analista Cuentas Pagar</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>215</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>salario_gerente_admin_conta</t>
+          <t>salario_jefe_produccion</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gerente Admin Conta</t>
+          <t>Jefe Produccion</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>185</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>salario_analista_cuentas_pagar</t>
+          <t>salario_ejecutivo_ventas</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Analista Cuentas Pagar</t>
+          <t>Ejecutivo Ventas</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>175</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>salario_empleado_administrativo</t>
+          <t>salario_gerente_admin_conta</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Empleado Administrativo</t>
+          <t>Gerente Admin Conta</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>175</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>salario_ejecutivo_ventas</t>
+          <t>salario_comprador_analista</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ejecutivo Ventas</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>175</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>salario_jefe_produccion</t>
+          <t>salario_analista_facturacion</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jefe Produccion</t>
+          <t>Analista Facturacion</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>165</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>salario_comprador_analista</t>
+          <t>salario_ceo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Ceo</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>160</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>salario_analista_facturacion</t>
+          <t>salario_jefe_rrhh</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Analista Facturacion</t>
+          <t>Jefe Rrhh</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>135</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>salario_jefe_ventas</t>
+          <t>salario_analista_admin_personal</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jefe Ventas</t>
+          <t>Analista Admin Personal</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>130</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>salario_jefe_compras</t>
+          <t>salario_gerente_planta</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Gerente Planta</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>125</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>salario_jefe_rrhh</t>
+          <t>salario_jefe_compras</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jefe Rrhh</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>125</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>salario_gerente_planta</t>
+          <t>salario_analista_cobranzas</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Gerente Planta</t>
+          <t>Analista Cobranzas</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>120</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>salario_gerente_ventas</t>
+          <t>salario_analista_logistica</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gerente Ventas</t>
+          <t>Analista Logistica</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>115</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>salario_analista_admin_personal</t>
+          <t>salario_responsable_liquidacion</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Analista Admin Personal</t>
+          <t>Responsable Liquidacion</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>115</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>salario_director_comercial</t>
+          <t>salario_jefe_ventas</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Director Comercial</t>
+          <t>Jefe Ventas</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>salario_analista_logistica</t>
+          <t>salario_gerente_rrhh</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Analista Logistica</t>
+          <t>Gerente Rrhh</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>salario_analista_cobranzas</t>
+          <t>salario_jefe_logistica</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Analista Cobranzas</t>
+          <t>Jefe Logistica</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>salario_responsable_liquidacion</t>
+          <t>salario_supervisor_produccion</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Responsable Liquidacion</t>
+          <t>Supervisor Produccion</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>105</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>salario_jefe_logistica</t>
+          <t>salario_tecnico_mantenimiento</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jefe Logistica</t>
+          <t>Tecnico Mantenimiento</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>105</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>salario_gerente_rrhh</t>
+          <t>salario_analista_control_gestion</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Gerente Rrhh</t>
+          <t>Analista Control Gestion</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>105</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>salario_analista_marketing</t>
+          <t>salario_jefe_calidad</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Analista Marketing</t>
+          <t>Jefe Calidad</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>100</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>salario_supervisor_produccion</t>
+          <t>salario_analista_marketing</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Supervisor Produccion</t>
+          <t>Analista Marketing</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>salario_tecnico_mantenimiento</t>
+          <t>salario_supervisor_depositos</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tecnico Mantenimiento</t>
+          <t>Supervisor Depositos</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>salario_jefe_calidad</t>
+          <t>salario_asistente_comex</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jefe Calidad</t>
+          <t>Asistente Comex</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>salario_analista_control_gestion</t>
+          <t>salario_jefe_finanzas</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Analista Control Gestion</t>
+          <t>Jefe Finanzas</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>salario_asistente_comex</t>
+          <t>salario_jefe_mantenimiento</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Asistente Comex</t>
+          <t>Jefe Mantenimiento</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>90</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>salario_jefe_mantenimiento</t>
+          <t>salario_supervisor_mantenimiento</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Jefe Mantenimiento</t>
+          <t>Supervisor Mantenimiento</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>90</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1885,17 +1887,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>{'No tenemos definido el aumento total para el 2025 (lo veremos mes a mes)': 105, '26 - 30%': 70, '21 - 25%': 55, '16 - 20 %': 50, '11 - 15%': 20, '31 - 35%': 20, '46 - 50%': 10, '6 - 10 %': 5, '36 - 40%': 5, '¿Qué % de AUMENTO SALARIAL estima dar la empresa en TODO el año 2025 (Ene - Dic) para empleados fuera de convenio?': 4}</t>
+          <t>{'No tenemos definido el aumento total para el 2025 (lo veremos mes a mes)': 21, '26 - 30%': 14, '21 - 25%': 11, '16 - 20 %': 10, '31 - 35%': 4, '11 - 15%': 4, '46 - 50%': 2, '36 - 40%': 1, '6 - 10 %': 1}</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'No esta definido todavía': 75, '4': 75, '3': 55, '2': 45, '12': 20, '9': 15, '1': 15, '6': 15, '7': 10, '10': 5, '5': 5, '8': 5, '¿Cuantos aumentos salariales estima dar en todo el año 2025 para empleados fuera de convenio?': 4}</t>
+          <t>{'No esta definido todavía': 15, '4': 15, '3': 11, '2': 9, '12': 4, '6': 3, '9': 3, '1': 3, '7': 2, '10': 1, '8': 1, '5': 1}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'1 - 5 %': 130, 'No medimos la Rotación de los empleados fuera de convenio': 60, '0% - No tuvimos Rotación de empleados fuera de convenio entre Enero y Agosto 2025': 50, '6 - 10 %': 35, '21 - 25%': 15, '26 - 30%': 15, '11 - 15%': 15, '16 - 20 %': 10, '&gt; 30%': 10, '¿Qué % Rotación tuvo la empresa entre Enero y Agosto 2025?  Indicador de entrada y salida de empleados (fuera de convenio). Incluye a todas las personas que dejan la organización (por renuncia, despido, jubilación, etc.) sobre el total de empleados. Indice de Rotación = Empleado que dejan la empresa / (empleados al inicio + empleados al final) / 2': 4}</t>
+          <t>{'1 - 5 %': 26, 'No medimos la Rotación de los empleados fuera de convenio': 12, '0% - No tuvimos Rotación de empleados fuera de convenio entre Enero y Agosto 2025': 10, '6 - 10 %': 7, '11 - 15%': 3, '21 - 25%': 3, '26 - 30%': 3, '&gt; 30%': 2, '16 - 20 %': 2}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Corregir clasificación Grande/Pyme hardcodeando índices de filas
- Filas 1-20 (índices 0-19): Grande (20 empresas)
- Filas 21-68 (índices 20+): Pyme (48 empresas)
- Eliminada lógica que calculaba desde columna "Dotación"
- Usar clasificación directa por índice de fila
- Regenerar datos normalizados y estadísticas con clasificación correcta

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/processed/estadisticas_salarios.xlsx
+++ b/data/processed/estadisticas_salarios.xlsx
@@ -509,40 +509,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" t="n">
         <v>2600000</v>
       </c>
       <c r="D2" t="n">
-        <v>2900000</v>
+        <v>2896210.5</v>
       </c>
       <c r="E2" t="n">
-        <v>3261187.5</v>
+        <v>3265593.75</v>
       </c>
       <c r="F2" t="n">
-        <v>3026340.651162791</v>
+        <v>3327883.652173913</v>
       </c>
       <c r="G2" t="n">
-        <v>2735000</v>
+        <v>2538999</v>
       </c>
       <c r="H2" t="n">
-        <v>3138000</v>
+        <v>2748715</v>
       </c>
       <c r="I2" t="n">
-        <v>3910000</v>
+        <v>3157640.5</v>
       </c>
       <c r="J2" t="n">
-        <v>2355996</v>
+        <v>2600000</v>
       </c>
       <c r="K2" t="n">
-        <v>2848000</v>
+        <v>3000000</v>
       </c>
       <c r="L2" t="n">
-        <v>3138000</v>
+        <v>3444000</v>
       </c>
       <c r="M2" t="n">
-        <v>10.18258426966292</v>
+        <v>-8.376166666666666</v>
       </c>
     </row>
     <row r="3">
@@ -552,814 +552,814 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" t="n">
-        <v>1540000</v>
+        <v>1520000</v>
       </c>
       <c r="D3" t="n">
         <v>1680000</v>
       </c>
       <c r="E3" t="n">
-        <v>1949999</v>
+        <v>1970703.5</v>
       </c>
       <c r="F3" t="n">
-        <v>1791032.43902439</v>
+        <v>1787816.023255814</v>
       </c>
       <c r="G3" t="n">
-        <v>1577800</v>
+        <v>1430231.25</v>
       </c>
       <c r="H3" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1693835</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1573960.5</v>
+      </c>
+      <c r="K3" t="n">
         <v>1800000</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1940999.25</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1538760.5</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1680000</v>
       </c>
       <c r="L3" t="n">
         <v>2045704</v>
       </c>
       <c r="M3" t="n">
-        <v>7.142857142857142</v>
+        <v>-11.11111111111111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Empleado Administrativo</t>
+          <t>Ceo</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C4" t="n">
-        <v>1164255</v>
+        <v>4841328.5</v>
       </c>
       <c r="D4" t="n">
-        <v>1270000</v>
+        <v>7100000</v>
       </c>
       <c r="E4" t="n">
-        <v>1400000</v>
+        <v>11104250</v>
       </c>
       <c r="F4" t="n">
-        <v>1308876.714285714</v>
+        <v>9415756.214285715</v>
       </c>
       <c r="G4" t="n">
-        <v>1227500</v>
+        <v>4062825</v>
       </c>
       <c r="H4" t="n">
-        <v>1296070</v>
+        <v>5902903.5</v>
       </c>
       <c r="I4" t="n">
-        <v>1325000</v>
+        <v>10444426.5</v>
       </c>
       <c r="J4" t="n">
-        <v>1164255</v>
+        <v>5058460.25</v>
       </c>
       <c r="K4" t="n">
-        <v>1270000</v>
+        <v>7970000</v>
       </c>
       <c r="L4" t="n">
-        <v>1407150</v>
+        <v>11158875</v>
       </c>
       <c r="M4" t="n">
-        <v>2.052755905511811</v>
+        <v>-25.9359661229611</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Analista Cuentas Pagar</t>
+          <t>Gerente Admin Conta</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C5" t="n">
-        <v>1404273.75</v>
+        <v>3600000</v>
       </c>
       <c r="D5" t="n">
-        <v>1600000</v>
+        <v>4500000</v>
       </c>
       <c r="E5" t="n">
-        <v>1714250</v>
+        <v>6246732</v>
       </c>
       <c r="F5" t="n">
-        <v>1596667.411764706</v>
+        <v>5134831.648648649</v>
       </c>
       <c r="G5" t="n">
-        <v>1476700</v>
+        <v>3696871</v>
       </c>
       <c r="H5" t="n">
-        <v>1600000</v>
+        <v>5100000</v>
       </c>
       <c r="I5" t="n">
-        <v>1720000</v>
+        <v>7000000</v>
       </c>
       <c r="J5" t="n">
-        <v>1385000</v>
+        <v>3184632.5</v>
       </c>
       <c r="K5" t="n">
-        <v>1600500</v>
+        <v>4470000</v>
       </c>
       <c r="L5" t="n">
-        <v>1816506.5</v>
+        <v>5618500</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.03124023742580443</v>
+        <v>14.09395973154362</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jefe Produccion</t>
+          <t>Analista Cuentas Pagar</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" t="n">
-        <v>2441880</v>
+        <v>1390000</v>
       </c>
       <c r="D6" t="n">
-        <v>2850000</v>
+        <v>1600000</v>
       </c>
       <c r="E6" t="n">
-        <v>3400000</v>
+        <v>1708500</v>
       </c>
       <c r="F6" t="n">
-        <v>3088920.181818182</v>
+        <v>1552191.2</v>
       </c>
       <c r="G6" t="n">
-        <v>2900000</v>
+        <v>1458547.5</v>
       </c>
       <c r="H6" t="n">
-        <v>3300000</v>
+        <v>1572076</v>
       </c>
       <c r="I6" t="n">
-        <v>3900000</v>
+        <v>1636000</v>
       </c>
       <c r="J6" t="n">
-        <v>2241741.5</v>
+        <v>1377700.5</v>
       </c>
       <c r="K6" t="n">
-        <v>2803973</v>
+        <v>1600500</v>
       </c>
       <c r="L6" t="n">
-        <v>3316000</v>
+        <v>1740000</v>
       </c>
       <c r="M6" t="n">
-        <v>17.69014894223304</v>
+        <v>-1.775945017182131</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ejecutivo Ventas</t>
+          <t>Empleado Administrativo</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" t="n">
-        <v>1638520</v>
+        <v>1164255</v>
       </c>
       <c r="D7" t="n">
-        <v>1992720.5</v>
+        <v>1270000</v>
       </c>
       <c r="E7" t="n">
-        <v>3025000</v>
+        <v>1400000</v>
       </c>
       <c r="F7" t="n">
-        <v>2392020.78125</v>
+        <v>1308876.714285714</v>
       </c>
       <c r="G7" t="n">
-        <v>1850000</v>
+        <v>1145750</v>
       </c>
       <c r="H7" t="n">
-        <v>2200000</v>
+        <v>1198524</v>
       </c>
       <c r="I7" t="n">
-        <v>3100000</v>
+        <v>1321250</v>
       </c>
       <c r="J7" t="n">
-        <v>1600000</v>
+        <v>1200000</v>
       </c>
       <c r="K7" t="n">
-        <v>1894257.5</v>
+        <v>1300000</v>
       </c>
       <c r="L7" t="n">
-        <v>3025000</v>
+        <v>1427768</v>
       </c>
       <c r="M7" t="n">
-        <v>16.14049304278853</v>
+        <v>-7.805846153846153</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Gerente Admin Conta</t>
+          <t>Ejecutivo Ventas</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C8" t="n">
-        <v>4191113.5</v>
+        <v>1600000</v>
       </c>
       <c r="D8" t="n">
-        <v>4760326</v>
+        <v>1900000</v>
       </c>
       <c r="E8" t="n">
-        <v>6711107</v>
+        <v>3000000</v>
       </c>
       <c r="F8" t="n">
-        <v>5729025.870967742</v>
+        <v>2317876.142857143</v>
       </c>
       <c r="G8" t="n">
-        <v>4440000</v>
+        <v>1636680</v>
       </c>
       <c r="H8" t="n">
-        <v>5235000</v>
+        <v>2444644</v>
       </c>
       <c r="I8" t="n">
-        <v>6922214</v>
+        <v>2971453.5</v>
       </c>
       <c r="J8" t="n">
-        <v>4075000</v>
+        <v>1592500</v>
       </c>
       <c r="K8" t="n">
-        <v>4522050</v>
+        <v>1853614.5</v>
       </c>
       <c r="L8" t="n">
-        <v>6310049</v>
+        <v>3000000</v>
       </c>
       <c r="M8" t="n">
-        <v>15.76607954356984</v>
+        <v>31.88524366851899</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Jefe Produccion</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="n">
-        <v>1546090</v>
+        <v>2441880</v>
       </c>
       <c r="D9" t="n">
-        <v>1652000</v>
+        <v>2850000</v>
       </c>
       <c r="E9" t="n">
-        <v>2000000</v>
+        <v>3400000</v>
       </c>
       <c r="F9" t="n">
-        <v>1921889.580645161</v>
+        <v>3088920.181818182</v>
       </c>
       <c r="G9" t="n">
-        <v>1600000</v>
+        <v>2731255.25</v>
       </c>
       <c r="H9" t="n">
-        <v>1692000</v>
+        <v>2825000</v>
       </c>
       <c r="I9" t="n">
-        <v>1900000</v>
+        <v>3003012</v>
       </c>
       <c r="J9" t="n">
-        <v>1544135</v>
+        <v>2179102</v>
       </c>
       <c r="K9" t="n">
-        <v>1641285</v>
+        <v>3300000</v>
       </c>
       <c r="L9" t="n">
-        <v>1975000</v>
+        <v>4000000</v>
       </c>
       <c r="M9" t="n">
-        <v>3.089956954459463</v>
+        <v>-14.39393939393939</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Analista Facturacion</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>1367990.5</v>
+        <v>1548045</v>
       </c>
       <c r="D10" t="n">
-        <v>1500000</v>
+        <v>1672000</v>
       </c>
       <c r="E10" t="n">
-        <v>1656000</v>
+        <v>2025000</v>
       </c>
       <c r="F10" t="n">
-        <v>1514282.518518518</v>
+        <v>2436894.59375</v>
       </c>
       <c r="G10" t="n">
-        <v>1391294.5</v>
+        <v>1493837.5</v>
       </c>
       <c r="H10" t="n">
-        <v>1490000</v>
+        <v>1571090</v>
       </c>
       <c r="I10" t="n">
-        <v>1605000</v>
+        <v>1697927.5</v>
       </c>
       <c r="J10" t="n">
-        <v>1331847</v>
+        <v>1573496.5</v>
       </c>
       <c r="K10" t="n">
-        <v>1400000</v>
+        <v>1779452.5</v>
       </c>
       <c r="L10" t="n">
-        <v>1645500</v>
+        <v>2155425</v>
       </c>
       <c r="M10" t="n">
-        <v>6.428571428571428</v>
+        <v>-11.70936004192301</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ceo</t>
+          <t>Analista Facturacion</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" t="n">
-        <v>7227500</v>
+        <v>1389458</v>
       </c>
       <c r="D11" t="n">
-        <v>10080000</v>
+        <v>1560065</v>
       </c>
       <c r="E11" t="n">
-        <v>12750000</v>
+        <v>1800000</v>
       </c>
       <c r="F11" t="n">
-        <v>12526837.23076923</v>
+        <v>1651319.555555556</v>
       </c>
       <c r="G11" t="n">
-        <v>10678875</v>
+        <v>1545048.75</v>
       </c>
       <c r="H11" t="n">
-        <v>15817750</v>
+        <v>1656000</v>
       </c>
       <c r="I11" t="n">
-        <v>26722374.5</v>
+        <v>1865125</v>
       </c>
       <c r="J11" t="n">
-        <v>6875000</v>
+        <v>1360401.5</v>
       </c>
       <c r="K11" t="n">
-        <v>8630000</v>
+        <v>1480000</v>
       </c>
       <c r="L11" t="n">
-        <v>11569500</v>
+        <v>1782400</v>
       </c>
       <c r="M11" t="n">
-        <v>83.28794901506373</v>
+        <v>11.89189189189189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jefe Rrhh</t>
+          <t>Jefe Ventas</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="n">
-        <v>2146466</v>
+        <v>2300000</v>
       </c>
       <c r="D12" t="n">
-        <v>2580000</v>
+        <v>2742000</v>
       </c>
       <c r="E12" t="n">
+        <v>3817527.5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3141387.423076923</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2209000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2684000</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2855012</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2300000</v>
+      </c>
+      <c r="K12" t="n">
         <v>3000000</v>
       </c>
-      <c r="F12" t="n">
-        <v>2930120</v>
-      </c>
-      <c r="G12" t="n">
-        <v>2437238</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2580000</v>
-      </c>
-      <c r="I12" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="J12" t="n">
-        <v>2031332</v>
-      </c>
-      <c r="K12" t="n">
-        <v>2287700</v>
-      </c>
       <c r="L12" t="n">
-        <v>2750000</v>
+        <v>4400100</v>
       </c>
       <c r="M12" t="n">
-        <v>12.77702495956638</v>
+        <v>-10.53333333333333</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Analista Admin Personal</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" t="n">
-        <v>1475000</v>
+        <v>2367000</v>
       </c>
       <c r="D13" t="n">
-        <v>1573407</v>
+        <v>2825000</v>
       </c>
       <c r="E13" t="n">
-        <v>1800000</v>
+        <v>3560000</v>
       </c>
       <c r="F13" t="n">
-        <v>1610904.52173913</v>
+        <v>2972496.84</v>
       </c>
       <c r="G13" t="n">
-        <v>1551750</v>
+        <v>2394352.75</v>
       </c>
       <c r="H13" t="n">
-        <v>1636703.5</v>
+        <v>2854035.5</v>
       </c>
       <c r="I13" t="n">
-        <v>1800000</v>
+        <v>3382665</v>
       </c>
       <c r="J13" t="n">
-        <v>1350000</v>
+        <v>2372734.5</v>
       </c>
       <c r="K13" t="n">
-        <v>1570354</v>
+        <v>2825000</v>
       </c>
       <c r="L13" t="n">
-        <v>1624489</v>
+        <v>3665662.5</v>
       </c>
       <c r="M13" t="n">
-        <v>4.225130129894278</v>
+        <v>1.027805309734513</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Gerente Planta</t>
+          <t>Jefe Rrhh</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" t="n">
-        <v>4157500</v>
+        <v>2146466</v>
       </c>
       <c r="D14" t="n">
-        <v>5000000</v>
+        <v>2580000</v>
       </c>
       <c r="E14" t="n">
-        <v>6740732.5</v>
+        <v>3000000</v>
       </c>
       <c r="F14" t="n">
-        <v>5967663.478260869</v>
+        <v>2930120</v>
       </c>
       <c r="G14" t="n">
-        <v>4798750</v>
+        <v>2173499</v>
       </c>
       <c r="H14" t="n">
-        <v>7000000</v>
+        <v>2675000</v>
       </c>
       <c r="I14" t="n">
-        <v>11296747</v>
+        <v>2927750</v>
       </c>
       <c r="J14" t="n">
-        <v>3523651.25</v>
+        <v>2162784</v>
       </c>
       <c r="K14" t="n">
-        <v>4595827.5</v>
+        <v>2543000</v>
       </c>
       <c r="L14" t="n">
-        <v>5744937.5</v>
+        <v>3150000</v>
       </c>
       <c r="M14" t="n">
-        <v>52.31207002438624</v>
+        <v>5.190719622493118</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Gerente Planta</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" t="n">
-        <v>2767514</v>
+        <v>3882883.75</v>
       </c>
       <c r="D15" t="n">
-        <v>3030660</v>
+        <v>4850000</v>
       </c>
       <c r="E15" t="n">
-        <v>3638705.5</v>
+        <v>6632348.75</v>
       </c>
       <c r="F15" t="n">
-        <v>3194667.652173913</v>
+        <v>5674844.166666667</v>
       </c>
       <c r="G15" t="n">
-        <v>2750000</v>
+        <v>3531535</v>
       </c>
       <c r="H15" t="n">
-        <v>3260000</v>
+        <v>5000000</v>
       </c>
       <c r="I15" t="n">
-        <v>3500000</v>
+        <v>6523965</v>
       </c>
       <c r="J15" t="n">
-        <v>2576014</v>
+        <v>4157500</v>
       </c>
       <c r="K15" t="n">
-        <v>3020918</v>
+        <v>4495000</v>
       </c>
       <c r="L15" t="n">
-        <v>3580000</v>
+        <v>6256250</v>
       </c>
       <c r="M15" t="n">
-        <v>7.914216804295912</v>
+        <v>11.23470522803115</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Analista Cobranzas</t>
+          <t>Gerente Ventas</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="n">
-        <v>1353796.25</v>
+        <v>3925000</v>
       </c>
       <c r="D16" t="n">
-        <v>1514050</v>
+        <v>5122000</v>
       </c>
       <c r="E16" t="n">
-        <v>1798506.5</v>
+        <v>6821107</v>
       </c>
       <c r="F16" t="n">
-        <v>1580097.318181818</v>
+        <v>5946885.869565218</v>
       </c>
       <c r="G16" t="n">
-        <v>1385000</v>
+        <v>3478915</v>
       </c>
       <c r="H16" t="n">
-        <v>1600000</v>
+        <v>4470000</v>
       </c>
       <c r="I16" t="n">
-        <v>1616500</v>
+        <v>6647851</v>
       </c>
       <c r="J16" t="n">
-        <v>1348532</v>
+        <v>4375000</v>
       </c>
       <c r="K16" t="n">
-        <v>1464434</v>
+        <v>5161000</v>
       </c>
       <c r="L16" t="n">
-        <v>1870000</v>
+        <v>6770553.5</v>
       </c>
       <c r="M16" t="n">
-        <v>9.25722838994451</v>
+        <v>-13.3888781243945</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Analista Logistica</t>
+          <t>Analista Admin Personal</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" t="n">
-        <v>1300000</v>
+        <v>1475000</v>
       </c>
       <c r="D17" t="n">
-        <v>1600000</v>
+        <v>1573407</v>
       </c>
       <c r="E17" t="n">
-        <v>1900000</v>
+        <v>1800000</v>
       </c>
       <c r="F17" t="n">
-        <v>1762187.285714286</v>
+        <v>1610904.52173913</v>
       </c>
       <c r="G17" t="n">
-        <v>1300000</v>
+        <v>1575000</v>
       </c>
       <c r="H17" t="n">
-        <v>1573400</v>
+        <v>1700000</v>
       </c>
       <c r="I17" t="n">
-        <v>1600000</v>
+        <v>1800000</v>
       </c>
       <c r="J17" t="n">
-        <v>1407687.5</v>
+        <v>1435280</v>
       </c>
       <c r="K17" t="n">
-        <v>1680392</v>
+        <v>1570354</v>
       </c>
       <c r="L17" t="n">
-        <v>1875000</v>
+        <v>1750000</v>
       </c>
       <c r="M17" t="n">
-        <v>-6.367085775223877</v>
+        <v>8.255845497257306</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Responsable Liquidacion</t>
+          <t>Director Comercial</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" t="n">
-        <v>1863500</v>
+        <v>4449225</v>
       </c>
       <c r="D18" t="n">
-        <v>2200000</v>
+        <v>5700000</v>
       </c>
       <c r="E18" t="n">
-        <v>2614457</v>
+        <v>10576750</v>
       </c>
       <c r="F18" t="n">
-        <v>2362442.666666667</v>
+        <v>7956053.681818182</v>
       </c>
       <c r="G18" t="n">
-        <v>2062500</v>
+        <v>6545250</v>
       </c>
       <c r="H18" t="n">
-        <v>2200000</v>
+        <v>9440500</v>
       </c>
       <c r="I18" t="n">
-        <v>2693750</v>
+        <v>10451750</v>
       </c>
       <c r="J18" t="n">
-        <v>1741602</v>
+        <v>4261725</v>
       </c>
       <c r="K18" t="n">
-        <v>2002305</v>
+        <v>5285000</v>
       </c>
       <c r="L18" t="n">
-        <v>2270000</v>
+        <v>10350000</v>
       </c>
       <c r="M18" t="n">
-        <v>9.873370939991661</v>
+        <v>78.62819299905392</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jefe Ventas</t>
+          <t>Analista Logistica</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C19" t="n">
-        <v>2519750</v>
+        <v>1300000</v>
       </c>
       <c r="D19" t="n">
-        <v>3225022.5</v>
+        <v>1588756</v>
       </c>
       <c r="E19" t="n">
-        <v>4300050</v>
+        <v>1875000</v>
       </c>
       <c r="F19" t="n">
-        <v>3578490.85</v>
+        <v>1721860.590909091</v>
       </c>
       <c r="G19" t="n">
-        <v>2900000</v>
+        <v>1630196</v>
       </c>
       <c r="H19" t="n">
-        <v>4200000</v>
+        <v>1760392</v>
       </c>
       <c r="I19" t="n">
-        <v>5000000</v>
+        <v>2007830.25</v>
       </c>
       <c r="J19" t="n">
-        <v>2336126.5</v>
+        <v>1275000</v>
       </c>
       <c r="K19" t="n">
-        <v>2684000</v>
+        <v>1502075</v>
       </c>
       <c r="L19" t="n">
-        <v>3662735</v>
+        <v>1825000</v>
       </c>
       <c r="M19" t="n">
-        <v>56.48286140089419</v>
+        <v>17.19734367458349</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Gerente Rrhh</t>
+          <t>Analista Cobranzas</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C20" t="n">
-        <v>3350311.5</v>
+        <v>1353796.25</v>
       </c>
       <c r="D20" t="n">
-        <v>4823000</v>
+        <v>1514050</v>
       </c>
       <c r="E20" t="n">
-        <v>6887500</v>
+        <v>1798506.5</v>
       </c>
       <c r="F20" t="n">
-        <v>5234530.1</v>
+        <v>1580097.318181818</v>
       </c>
       <c r="G20" t="n">
-        <v>4200000</v>
+        <v>1600000</v>
       </c>
       <c r="H20" t="n">
-        <v>4300126</v>
+        <v>1623404</v>
       </c>
       <c r="I20" t="n">
-        <v>7700000</v>
+        <v>1870000</v>
       </c>
       <c r="J20" t="n">
-        <v>3127500</v>
+        <v>1300000</v>
       </c>
       <c r="K20" t="n">
-        <v>4061100</v>
+        <v>1464434</v>
       </c>
       <c r="L20" t="n">
-        <v>6019573.5</v>
+        <v>1625000</v>
       </c>
       <c r="M20" t="n">
-        <v>5.885745241437049</v>
+        <v>10.85538849821842</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jefe Logistica</t>
+          <t>Responsable Liquidacion</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" t="n">
-        <v>2296597.5</v>
+        <v>1863500</v>
       </c>
       <c r="D21" t="n">
-        <v>2840897.5</v>
+        <v>2200000</v>
       </c>
       <c r="E21" t="n">
-        <v>3320583.5</v>
+        <v>2614457</v>
       </c>
       <c r="F21" t="n">
-        <v>3067139.45</v>
+        <v>2362442.666666667</v>
       </c>
       <c r="G21" t="n">
+        <v>1967603.75</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2171718</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2405000</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="K21" t="n">
         <v>2200000</v>
       </c>
-      <c r="H21" t="n">
-        <v>2500000</v>
-      </c>
-      <c r="I21" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="J21" t="n">
-        <v>2500000</v>
-      </c>
-      <c r="K21" t="n">
-        <v>2866795</v>
-      </c>
       <c r="L21" t="n">
-        <v>3552281</v>
+        <v>2769806</v>
       </c>
       <c r="M21" t="n">
-        <v>-12.79460163701974</v>
+        <v>-1.285545454545455</v>
       </c>
     </row>
   </sheetData>
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -1425,322 +1425,322 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>salario_empleado_administrativo</t>
+          <t>salario_ceo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Empleado Administrativo</t>
+          <t>Ceo</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>salario_analista_cuentas_pagar</t>
+          <t>salario_gerente_admin_conta</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Analista Cuentas Pagar</t>
+          <t>Gerente Admin Conta</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>salario_jefe_produccion</t>
+          <t>salario_analista_cuentas_pagar</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jefe Produccion</t>
+          <t>Analista Cuentas Pagar</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>salario_ejecutivo_ventas</t>
+          <t>salario_empleado_administrativo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ejecutivo Ventas</t>
+          <t>Empleado Administrativo</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>salario_gerente_admin_conta</t>
+          <t>salario_ejecutivo_ventas</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gerente Admin Conta</t>
+          <t>Ejecutivo Ventas</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>salario_comprador_analista</t>
+          <t>salario_jefe_produccion</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Jefe Produccion</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>salario_analista_facturacion</t>
+          <t>salario_comprador_analista</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Analista Facturacion</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>salario_ceo</t>
+          <t>salario_analista_facturacion</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ceo</t>
+          <t>Analista Facturacion</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>salario_jefe_rrhh</t>
+          <t>salario_jefe_ventas</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jefe Rrhh</t>
+          <t>Jefe Ventas</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>salario_analista_admin_personal</t>
+          <t>salario_jefe_compras</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Analista Admin Personal</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>salario_gerente_planta</t>
+          <t>salario_jefe_rrhh</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gerente Planta</t>
+          <t>Jefe Rrhh</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>salario_jefe_compras</t>
+          <t>salario_gerente_planta</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Gerente Planta</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>salario_analista_cobranzas</t>
+          <t>salario_gerente_ventas</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Analista Cobranzas</t>
+          <t>Gerente Ventas</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>salario_analista_logistica</t>
+          <t>salario_analista_admin_personal</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Analista Logistica</t>
+          <t>Analista Admin Personal</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>salario_responsable_liquidacion</t>
+          <t>salario_director_comercial</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Responsable Liquidacion</t>
+          <t>Director Comercial</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>salario_jefe_ventas</t>
+          <t>salario_analista_logistica</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jefe Ventas</t>
+          <t>Analista Logistica</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>salario_gerente_rrhh</t>
+          <t>salario_analista_cobranzas</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Gerente Rrhh</t>
+          <t>Analista Cobranzas</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>salario_jefe_logistica</t>
+          <t>salario_responsable_liquidacion</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jefe Logistica</t>
+          <t>Responsable Liquidacion</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>salario_supervisor_produccion</t>
+          <t>salario_jefe_logistica</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Supervisor Produccion</t>
+          <t>Jefe Logistica</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>salario_tecnico_mantenimiento</t>
+          <t>salario_gerente_rrhh</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tecnico Mantenimiento</t>
+          <t>Gerente Rrhh</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>salario_analista_control_gestion</t>
+          <t>salario_analista_marketing</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Analista Control Gestion</t>
+          <t>Analista Marketing</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
@@ -1761,91 +1761,91 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>salario_analista_marketing</t>
+          <t>salario_supervisor_produccion</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Analista Marketing</t>
+          <t>Supervisor Produccion</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>salario_supervisor_depositos</t>
+          <t>salario_tecnico_mantenimiento</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Supervisor Depositos</t>
+          <t>Tecnico Mantenimiento</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>salario_asistente_comex</t>
+          <t>salario_analista_control_gestion</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Asistente Comex</t>
+          <t>Analista Control Gestion</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>salario_jefe_finanzas</t>
+          <t>salario_jefe_mantenimiento</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Jefe Finanzas</t>
+          <t>Jefe Mantenimiento</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>salario_jefe_mantenimiento</t>
+          <t>salario_asistente_comex</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jefe Mantenimiento</t>
+          <t>Asistente Comex</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>salario_supervisor_mantenimiento</t>
+          <t>salario_supervisor_depositos</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Supervisor Mantenimiento</t>
+          <t>Supervisor Depositos</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1887,17 +1887,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>{'No tenemos definido el aumento total para el 2025 (lo veremos mes a mes)': 21, '26 - 30%': 14, '21 - 25%': 11, '16 - 20 %': 10, '31 - 35%': 4, '11 - 15%': 4, '46 - 50%': 2, '36 - 40%': 1, '6 - 10 %': 1}</t>
+          <t>{'No tenemos definido el aumento total para el 2025 (lo veremos mes a mes)': 21, '26 - 30%': 14, '21 - 25%': 11, '16 - 20 %': 10, '11 - 15%': 4, '31 - 35%': 4, '46 - 50%': 2, '6 - 10 %': 1, '36 - 40%': 1}</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'No esta definido todavía': 15, '4': 15, '3': 11, '2': 9, '12': 4, '6': 3, '9': 3, '1': 3, '7': 2, '10': 1, '8': 1, '5': 1}</t>
+          <t>{'No esta definido todavía': 15, '4': 15, '3': 11, '2': 9, '12': 4, '9': 3, '1': 3, '6': 3, '7': 2, '10': 1, '5': 1, '8': 1}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'1 - 5 %': 26, 'No medimos la Rotación de los empleados fuera de convenio': 12, '0% - No tuvimos Rotación de empleados fuera de convenio entre Enero y Agosto 2025': 10, '6 - 10 %': 7, '11 - 15%': 3, '21 - 25%': 3, '26 - 30%': 3, '&gt; 30%': 2, '16 - 20 %': 2}</t>
+          <t>{'1 - 5 %': 26, 'No medimos la Rotación de los empleados fuera de convenio': 12, '0% - No tuvimos Rotación de empleados fuera de convenio entre Enero y Agosto 2025': 10, '6 - 10 %': 7, '21 - 25%': 3, '26 - 30%': 3, '11 - 15%': 3, '16 - 20 %': 2, '&gt; 30%': 2}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature: Actualizar a nuevadata.csv con clasificación correcta
- Reemplazar encuesta_salarial.csv con nuevadata.csv
- Usar separador ; (punto y coma) en CSV
- Clasificación: Filas 1-18 Grande, Filas 19+ Pyme
- Mantener 0s como valores válidos (no convertir a NaN)
- Total: 18 Grandes, 50 Pymes (68 empresas)
- Regenerar datos normalizados y estadísticas

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/processed/estadisticas_salarios.xlsx
+++ b/data/processed/estadisticas_salarios.xlsx
@@ -505,733 +505,711 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jefe Admin Conta</t>
+          <t>Ingeniero Agronomo</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C2" t="n">
-        <v>2600000</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2896210.5</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>3265593.75</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3327883.652173913</v>
+        <v>552062.2941176471</v>
       </c>
       <c r="G2" t="n">
-        <v>2538999</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>2748715</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>3157640.5</v>
+        <v>2137500</v>
       </c>
       <c r="J2" t="n">
-        <v>2600000</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>3444000</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-8.376166666666666</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Analista Contabilidad</t>
+          <t>Director Comercial</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C3" t="n">
-        <v>1520000</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1680000</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1970703.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1787816.023255814</v>
+        <v>2162071.073529412</v>
       </c>
       <c r="G3" t="n">
-        <v>1430231.25</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1600000</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1693835</v>
+        <v>8900000</v>
       </c>
       <c r="J3" t="n">
-        <v>1573960.5</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>1800000</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2045704</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-11.11111111111111</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ceo</t>
+          <t>Gerente Seguridad</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C4" t="n">
-        <v>4841328.5</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>7100000</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>11104250</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>9415756.214285715</v>
+        <v>348298.1176470588</v>
       </c>
       <c r="G4" t="n">
-        <v>4062825</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>5902903.5</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>10444426.5</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>5058460.25</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>7970000</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>11158875</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-25.9359661229611</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gerente Admin Conta</t>
+          <t>Responsable Sustentabilidad</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C5" t="n">
-        <v>3600000</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>4500000</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>6246732</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>5134831.648648649</v>
+        <v>459135.1176470588</v>
       </c>
       <c r="G5" t="n">
-        <v>3696871</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>5100000</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>7000000</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>3184632.5</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>4470000</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>5618500</v>
-      </c>
-      <c r="M5" t="n">
-        <v>14.09395973154362</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Analista Cuentas Pagar</t>
+          <t>Diseñador Grafico</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C6" t="n">
-        <v>1390000</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1600000</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1708500</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1552191.2</v>
+        <v>288778.4117647059</v>
       </c>
       <c r="G6" t="n">
-        <v>1458547.5</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1572076</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1636000</v>
+        <v>600000</v>
       </c>
       <c r="J6" t="n">
-        <v>1377700.5</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>1600500</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1740000</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-1.775945017182131</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Empleado Administrativo</t>
+          <t>Tecnico Calidad</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C7" t="n">
-        <v>1164255</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1270000</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1308876.714285714</v>
+        <v>105432.4852941177</v>
       </c>
       <c r="G7" t="n">
-        <v>1145750</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>1198524</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>1321250</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>1300000</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1427768</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-7.805846153846153</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ejecutivo Ventas</t>
+          <t>Analista Calidad</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C8" t="n">
-        <v>1600000</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1900000</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2317876.142857143</v>
+        <v>296276.8970588236</v>
       </c>
       <c r="G8" t="n">
-        <v>1636680</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>2444644</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>2971453.5</v>
+        <v>1334954.5</v>
       </c>
       <c r="J8" t="n">
-        <v>1592500</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1853614.5</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="M8" t="n">
-        <v>31.88524366851899</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jefe Produccion</t>
+          <t>Jefe Calidad</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C9" t="n">
-        <v>2441880</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2850000</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>3400000</v>
+        <v>1902500</v>
       </c>
       <c r="F9" t="n">
-        <v>3088920.181818182</v>
+        <v>740034.0441176471</v>
       </c>
       <c r="G9" t="n">
-        <v>2731255.25</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>2825000</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>3003012</v>
+        <v>2502500</v>
       </c>
       <c r="J9" t="n">
-        <v>2179102</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>3300000</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-14.39393939393939</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Gerente Calidad</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="C10" t="n">
-        <v>1548045</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1672000</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>2025000</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2436894.59375</v>
+        <v>409096.8529411764</v>
       </c>
       <c r="G10" t="n">
-        <v>1493837.5</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>1571090</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>1697927.5</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>1573496.5</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>1779452.5</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>2155425</v>
-      </c>
-      <c r="M10" t="n">
-        <v>-11.70936004192301</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Analista Facturacion</t>
+          <t>Tecnico Mantenimiento</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C11" t="n">
-        <v>1389458</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1560065</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1800000</v>
+        <v>1225000</v>
       </c>
       <c r="F11" t="n">
-        <v>1651319.555555556</v>
+        <v>444247.4411764706</v>
       </c>
       <c r="G11" t="n">
-        <v>1545048.75</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1656000</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1865125</v>
+        <v>1450000</v>
       </c>
       <c r="J11" t="n">
-        <v>1360401.5</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1480000</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>1782400</v>
-      </c>
-      <c r="M11" t="n">
-        <v>11.89189189189189</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jefe Ventas</t>
+          <t>Supervisor Mantenimiento</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C12" t="n">
-        <v>2300000</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>2742000</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>3817527.5</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>3141387.423076923</v>
+        <v>604682.5882352941</v>
       </c>
       <c r="G12" t="n">
-        <v>2209000</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>2684000</v>
+        <v>950000</v>
       </c>
       <c r="I12" t="n">
-        <v>2855012</v>
+        <v>2210202.75</v>
       </c>
       <c r="J12" t="n">
-        <v>2300000</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>4400100</v>
-      </c>
-      <c r="M12" t="n">
-        <v>-10.53333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Jefe Mantenimiento</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C13" t="n">
-        <v>2367000</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>2825000</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>3560000</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>2972496.84</v>
+        <v>673238.9117647059</v>
       </c>
       <c r="G13" t="n">
-        <v>2394352.75</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>2854035.5</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>3382665</v>
+        <v>2590783.75</v>
       </c>
       <c r="J13" t="n">
-        <v>2372734.5</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>2825000</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>3665662.5</v>
-      </c>
-      <c r="M13" t="n">
-        <v>1.027805309734513</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jefe Rrhh</t>
+          <t>Gerente Mantenimiento</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C14" t="n">
-        <v>2146466</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>2580000</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>2930120</v>
+        <v>652022.5147058824</v>
       </c>
       <c r="G14" t="n">
-        <v>2173499</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>2675000</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>2927750</v>
+        <v>2100000</v>
       </c>
       <c r="J14" t="n">
-        <v>2162784</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>2543000</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>3150000</v>
-      </c>
-      <c r="M14" t="n">
-        <v>5.190719622493118</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gerente Planta</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C15" t="n">
-        <v>3882883.75</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>4850000</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>6632348.75</v>
+        <v>1608392.5</v>
       </c>
       <c r="F15" t="n">
-        <v>5674844.166666667</v>
+        <v>876155.5441176471</v>
       </c>
       <c r="G15" t="n">
-        <v>3531535</v>
+        <v>365837.5</v>
       </c>
       <c r="H15" t="n">
-        <v>5000000</v>
+        <v>1582000</v>
       </c>
       <c r="I15" t="n">
-        <v>6523965</v>
+        <v>1880375</v>
       </c>
       <c r="J15" t="n">
-        <v>4157500</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>4495000</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>6256250</v>
-      </c>
-      <c r="M15" t="n">
-        <v>11.23470522803115</v>
+        <v>1548045</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Gerente Ventas</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C16" t="n">
-        <v>3925000</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>5122000</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>6821107</v>
+        <v>2758757</v>
       </c>
       <c r="F16" t="n">
-        <v>5946885.869565218</v>
+        <v>1080549.352941176</v>
       </c>
       <c r="G16" t="n">
-        <v>3478915</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>4470000</v>
+        <v>2787500</v>
       </c>
       <c r="I16" t="n">
-        <v>6647851</v>
+        <v>3450000</v>
       </c>
       <c r="J16" t="n">
-        <v>4375000</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>5161000</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>6770553.5</v>
-      </c>
-      <c r="M16" t="n">
-        <v>-13.3888781243945</v>
+        <v>0</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Analista Admin Personal</t>
+          <t>Gerente Compras</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C17" t="n">
-        <v>1475000</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>1573407</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1800000</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1610904.52173913</v>
+        <v>501945.6911764706</v>
       </c>
       <c r="G17" t="n">
-        <v>1575000</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>1700000</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>1800000</v>
+        <v>2325000</v>
       </c>
       <c r="J17" t="n">
-        <v>1435280</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>1570354</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>1750000</v>
-      </c>
-      <c r="M17" t="n">
-        <v>8.255845497257306</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Director Comercial</t>
+          <t>Supervisor Depositos</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C18" t="n">
-        <v>4449225</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>5700000</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>10576750</v>
+        <v>351875</v>
       </c>
       <c r="F18" t="n">
-        <v>7956053.681818182</v>
+        <v>571177.2352941176</v>
       </c>
       <c r="G18" t="n">
-        <v>6545250</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>9440500</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>10451750</v>
+        <v>1937270.75</v>
       </c>
       <c r="J18" t="n">
-        <v>4261725</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>5285000</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>10350000</v>
-      </c>
-      <c r="M18" t="n">
-        <v>78.62819299905392</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1240,127 +1218,121 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C19" t="n">
-        <v>1300000</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>1588756</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1875000</v>
+        <v>1225000</v>
       </c>
       <c r="F19" t="n">
-        <v>1721860.590909091</v>
+        <v>544204.8970588235</v>
       </c>
       <c r="G19" t="n">
-        <v>1630196</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>1760392</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>2007830.25</v>
+        <v>1275000</v>
       </c>
       <c r="J19" t="n">
-        <v>1275000</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>1502075</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>1825000</v>
-      </c>
-      <c r="M19" t="n">
-        <v>17.19734367458349</v>
-      </c>
+        <v>1003796.75</v>
+      </c>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Analista Cobranzas</t>
+          <t>Jefe Logistica</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C20" t="n">
-        <v>1353796.25</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>1514050</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1798506.5</v>
+        <v>2132500</v>
       </c>
       <c r="F20" t="n">
-        <v>1580097.318181818</v>
+        <v>902099.8382352941</v>
       </c>
       <c r="G20" t="n">
-        <v>1600000</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1623404</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>1870000</v>
+        <v>2264792.5</v>
       </c>
       <c r="J20" t="n">
-        <v>1300000</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>1464434</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>1625000</v>
-      </c>
-      <c r="M20" t="n">
-        <v>10.85538849821842</v>
-      </c>
+        <v>1474108.5</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Responsable Liquidacion</t>
+          <t>Jefe Planificacion</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C21" t="n">
-        <v>1863500</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>2200000</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>2614457</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>2362442.666666667</v>
+        <v>640254.7647058824</v>
       </c>
       <c r="G21" t="n">
-        <v>1967603.75</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>2171718</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>2405000</v>
+        <v>2614681.75</v>
       </c>
       <c r="J21" t="n">
-        <v>1800000</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>2200000</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>2769806</v>
-      </c>
-      <c r="M21" t="n">
-        <v>-1.285545454545455</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1401,256 +1373,256 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>salario_jefe_admin_conta</t>
+          <t>salario_ingeniero_agronomo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jefe Admin Conta</t>
+          <t>Ingeniero Agronomo</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>salario_analista_contabilidad</t>
+          <t>salario_director_comercial</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Analista Contabilidad</t>
+          <t>Director Comercial</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>salario_ceo</t>
+          <t>salario_gerente_seguridad</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ceo</t>
+          <t>Gerente Seguridad</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>salario_gerente_admin_conta</t>
+          <t>salario_responsable_sustentabilidad</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Gerente Admin Conta</t>
+          <t>Responsable Sustentabilidad</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>salario_analista_cuentas_pagar</t>
+          <t>salario_diseñador_grafico</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Analista Cuentas Pagar</t>
+          <t>Diseñador Grafico</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>salario_empleado_administrativo</t>
+          <t>salario_tecnico_calidad</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Empleado Administrativo</t>
+          <t>Tecnico Calidad</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>salario_ejecutivo_ventas</t>
+          <t>salario_analista_calidad</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ejecutivo Ventas</t>
+          <t>Analista Calidad</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>salario_jefe_produccion</t>
+          <t>salario_jefe_calidad</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jefe Produccion</t>
+          <t>Jefe Calidad</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>33</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>salario_comprador_analista</t>
+          <t>salario_gerente_calidad</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Gerente Calidad</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>salario_analista_facturacion</t>
+          <t>salario_tecnico_mantenimiento</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Analista Facturacion</t>
+          <t>Tecnico Mantenimiento</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>salario_jefe_ventas</t>
+          <t>salario_supervisor_mantenimiento</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jefe Ventas</t>
+          <t>Supervisor Mantenimiento</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>salario_jefe_compras</t>
+          <t>salario_jefe_mantenimiento</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Jefe Mantenimiento</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>salario_jefe_rrhh</t>
+          <t>salario_gerente_mantenimiento</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jefe Rrhh</t>
+          <t>Gerente Mantenimiento</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>salario_gerente_planta</t>
+          <t>salario_comprador_analista</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Gerente Planta</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>salario_gerente_ventas</t>
+          <t>salario_jefe_compras</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Gerente Ventas</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>salario_analista_admin_personal</t>
+          <t>salario_gerente_compras</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Analista Admin Personal</t>
+          <t>Gerente Compras</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>salario_director_comercial</t>
+          <t>salario_supervisor_depositos</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Director Comercial</t>
+          <t>Supervisor Depositos</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -1665,187 +1637,187 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>salario_analista_cobranzas</t>
+          <t>salario_jefe_logistica</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Analista Cobranzas</t>
+          <t>Jefe Logistica</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>salario_responsable_liquidacion</t>
+          <t>salario_jefe_planificacion</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Responsable Liquidacion</t>
+          <t>Jefe Planificacion</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>salario_jefe_logistica</t>
+          <t>salario_gerente_supply_chain</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jefe Logistica</t>
+          <t>Gerente Supply Chain</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>salario_gerente_rrhh</t>
+          <t>salario_analista_laboratorio</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Gerente Rrhh</t>
+          <t>Analista Laboratorio</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>salario_analista_marketing</t>
+          <t>salario_jefe_laboratorio</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Analista Marketing</t>
+          <t>Jefe Laboratorio</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>salario_jefe_calidad</t>
+          <t>salario_jefe_seguridad</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Jefe Calidad</t>
+          <t>Jefe Seguridad</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>salario_supervisor_produccion</t>
+          <t>salario_tecnico_seguridad</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Supervisor Produccion</t>
+          <t>Tecnico Seguridad</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>salario_tecnico_mantenimiento</t>
+          <t>salario_jefe_ingenieria</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tecnico Mantenimiento</t>
+          <t>Jefe Ingenieria</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>salario_analista_control_gestion</t>
+          <t>salario_analista_capacitacion</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Analista Control Gestion</t>
+          <t>Analista Capacitacion</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>salario_jefe_mantenimiento</t>
+          <t>salario_joven_profesional</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Jefe Mantenimiento</t>
+          <t>Joven Profesional</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>18</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>salario_asistente_comex</t>
+          <t>salario_analista_helpdesk</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Asistente Comex</t>
+          <t>Analista Helpdesk</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>18</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>salario_supervisor_depositos</t>
+          <t>salario_jefe_soporte</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Supervisor Depositos</t>
+          <t>Jefe Soporte</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1887,17 +1859,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>{'No tenemos definido el aumento total para el 2025 (lo veremos mes a mes)': 21, '26 - 30%': 14, '21 - 25%': 11, '16 - 20 %': 10, '11 - 15%': 4, '31 - 35%': 4, '46 - 50%': 2, '6 - 10 %': 1, '36 - 40%': 1}</t>
+          <t>{'No tenemos definido el aumento total para el 2025 (lo veremos mes a mes)': 21, '26 - 30%': 14, '21 - 25%': 11, '16 - 20 %': 10, '31 - 35%': 4, '11 - 15%': 4, '46 - 50%': 2, '36 - 40%': 1, '6 - 10 %': 1}</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'No esta definido todavía': 15, '4': 15, '3': 11, '2': 9, '12': 4, '9': 3, '1': 3, '6': 3, '7': 2, '10': 1, '5': 1, '8': 1}</t>
+          <t>{'No esta definido todavía': 15, '4': 15, '3': 11, '2': 9, '12': 4, '6': 3, '9': 3, '1': 3, '7': 2, '10': 1, '8': 1, '5': 1}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'1 - 5 %': 26, 'No medimos la Rotación de los empleados fuera de convenio': 12, '0% - No tuvimos Rotación de empleados fuera de convenio entre Enero y Agosto 2025': 10, '6 - 10 %': 7, '21 - 25%': 3, '26 - 30%': 3, '11 - 15%': 3, '16 - 20 %': 2, '&gt; 30%': 2}</t>
+          <t>{'1 - 5 %': 26, 'No medimos la Rotación de los empleados fuera de convenio': 12, '0% - No tuvimos Rotación de empleados fuera de convenio entre Enero y Agosto 2025': 10, '6 - 10 %': 7, '11 - 15%': 3, '21 - 25%': 3, '26 - 30%': 3, '&gt; 30%': 2, '16 - 20 %': 2}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Filtrar valores 0 en cálculos estadísticos
- Agregar filtro salarios > 0 en calcular_percentiles_cargo
- Los 0 representan datos faltantes, no deben incluirse en estadísticas
- Aplicar filtro tanto en segmentación por tamaño como en general
- Regenerar estadisticas_salarios.xlsx con cálculos correctos

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/processed/estadisticas_salarios.xlsx
+++ b/data/processed/estadisticas_salarios.xlsx
@@ -505,752 +505,776 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ingeniero Agronomo</t>
+          <t>Jefe Admin Conta</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2600000</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2900000</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>3261187.5</v>
       </c>
       <c r="F2" t="n">
-        <v>552062.2941176471</v>
+        <v>3026340.651162791</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>2733105.25</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3108281</v>
       </c>
       <c r="I2" t="n">
-        <v>2137500</v>
+        <v>3605000</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>2355996</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>2848000</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="inlineStr"/>
+        <v>3138000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>9.139080056179775</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Director Comercial</t>
+          <t>Analista Contabilidad</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1540000</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1680000</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1949999</v>
       </c>
       <c r="F3" t="n">
-        <v>2162071.073529412</v>
+        <v>1791032.43902439</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1547600</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1711000</v>
       </c>
       <c r="I3" t="n">
-        <v>8900000</v>
+        <v>1928002.5</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1538760.5</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1680000</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr"/>
+        <v>2045704</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.845238095238095</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Gerente Seguridad</t>
+          <t>Empleado Administrativo</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1164255</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1270000</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1400000</v>
       </c>
       <c r="F4" t="n">
-        <v>348298.1176470588</v>
+        <v>1308876.714285714</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1165286</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1281070</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1325000</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1164255</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1270000</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
+        <v>1407150</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8716535433070867</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Responsable Sustentabilidad</t>
+          <t>Analista Cuentas Pagar</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1404273.75</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1600000</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1714250</v>
       </c>
       <c r="F5" t="n">
-        <v>459135.1176470588</v>
+        <v>1596667.411764706</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1494175</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1553449.5</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1651000</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1385000</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1600500</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
+        <v>1816506.5</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-2.939737582005623</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Diseñador Grafico</t>
+          <t>Jefe Produccion</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>2441880</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>2850000</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>3400000</v>
       </c>
       <c r="F6" t="n">
-        <v>288778.4117647059</v>
+        <v>3088920.181818182</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>2687503.5</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>3300000</v>
       </c>
       <c r="I6" t="n">
-        <v>600000</v>
+        <v>3643744</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>2241741.5</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>2803973</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
+        <v>3316000</v>
+      </c>
+      <c r="M6" t="n">
+        <v>17.69014894223304</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tecnico Calidad</t>
+          <t>Ejecutivo Ventas</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1638520</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1992720.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3025000</v>
       </c>
       <c r="F7" t="n">
-        <v>105432.4852941177</v>
+        <v>2392020.78125</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1875000</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>2322322</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>3050000</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1600000</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1894257.5</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="inlineStr"/>
+        <v>3025000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>22.59801003823398</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Analista Calidad</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1546090</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1652000</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2000000</v>
       </c>
       <c r="F8" t="n">
-        <v>296276.8970588236</v>
+        <v>1921889.580645161</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1564000</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1692000</v>
       </c>
       <c r="I8" t="n">
-        <v>1334954.5</v>
+        <v>2000000</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>1544135</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1641285</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
+        <v>1975000</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3.089956954459463</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jefe Calidad</t>
+          <t>Gerente Admin Conta</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>4191113.5</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>4760326</v>
       </c>
       <c r="E9" t="n">
-        <v>1902500</v>
+        <v>6711107</v>
       </c>
       <c r="F9" t="n">
-        <v>740034.0441176471</v>
+        <v>5729025.870967742</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>4720000</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>5600000</v>
       </c>
       <c r="I9" t="n">
-        <v>2502500</v>
+        <v>6961107</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>4075000</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>4522050</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="inlineStr"/>
+        <v>6310049</v>
+      </c>
+      <c r="M9" t="n">
+        <v>23.83764000840327</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Gerente Calidad</t>
+          <t>Analista Facturacion</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1367990.5</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1500000</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1656000</v>
       </c>
       <c r="F10" t="n">
-        <v>409096.8529411764</v>
+        <v>1514282.518518518</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1460000</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1520000</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1657700</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1331847</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1400000</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
+        <v>1645500</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8.571428571428571</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tecnico Mantenimiento</t>
+          <t>Ceo</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>7227500</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>10080000</v>
       </c>
       <c r="E11" t="n">
-        <v>1225000</v>
+        <v>12750000</v>
       </c>
       <c r="F11" t="n">
-        <v>444247.4411764706</v>
+        <v>12526837.23076923</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>10997750</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>19722471</v>
       </c>
       <c r="I11" t="n">
-        <v>1450000</v>
+        <v>24481583</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>6875000</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>8630000</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="inlineStr"/>
+        <v>11569500</v>
+      </c>
+      <c r="M11" t="n">
+        <v>128.5338470451912</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Supervisor Mantenimiento</t>
+          <t>Jefe Rrhh</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>2146466</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2580000</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>3000000</v>
       </c>
       <c r="F12" t="n">
-        <v>604682.5882352941</v>
+        <v>2930120</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>2446809.5</v>
       </c>
       <c r="H12" t="n">
-        <v>950000</v>
+        <v>2600000</v>
       </c>
       <c r="I12" t="n">
-        <v>2210202.75</v>
+        <v>3350138.75</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>2031332</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>2287700</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>2750000</v>
+      </c>
+      <c r="M12" t="n">
+        <v>13.65126546312891</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jefe Mantenimiento</t>
+          <t>Gerente Planta</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>4157500</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>6740732.5</v>
       </c>
       <c r="F13" t="n">
-        <v>673238.9117647059</v>
+        <v>5967663.478260869</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>5227500</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>6000000</v>
       </c>
       <c r="I13" t="n">
-        <v>2590783.75</v>
+        <v>7811982.5</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>3523651.25</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>4595827.5</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="inlineStr"/>
+        <v>5744937.5</v>
+      </c>
+      <c r="M13" t="n">
+        <v>30.55320287804536</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Gerente Mantenimiento</t>
+          <t>Analista Admin Personal</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1475000</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1573407</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1800000</v>
       </c>
       <c r="F14" t="n">
-        <v>652022.5147058824</v>
+        <v>1610904.52173913</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1522500</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1636703.5</v>
       </c>
       <c r="I14" t="n">
-        <v>2100000</v>
+        <v>1800000</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>1350000</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>1570354</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="inlineStr"/>
+        <v>1624489</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4.225130129894278</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2767514</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>3030660</v>
       </c>
       <c r="E15" t="n">
-        <v>1608392.5</v>
+        <v>3638705.5</v>
       </c>
       <c r="F15" t="n">
-        <v>876155.5441176471</v>
+        <v>3194667.652173913</v>
       </c>
       <c r="G15" t="n">
-        <v>365837.5</v>
+        <v>2806250</v>
       </c>
       <c r="H15" t="n">
-        <v>1582000</v>
+        <v>3280000</v>
       </c>
       <c r="I15" t="n">
-        <v>1880375</v>
+        <v>3883058.25</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>2576014</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>3020918</v>
       </c>
       <c r="L15" t="n">
-        <v>1548045</v>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>3580000</v>
+      </c>
+      <c r="M15" t="n">
+        <v>8.57626721413822</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Analista Cobranzas</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1353796.25</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1514050</v>
       </c>
       <c r="E16" t="n">
-        <v>2758757</v>
+        <v>1798506.5</v>
       </c>
       <c r="F16" t="n">
-        <v>1080549.352941176</v>
+        <v>1580097.318181818</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1470000</v>
       </c>
       <c r="H16" t="n">
-        <v>2787500</v>
+        <v>1600000</v>
       </c>
       <c r="I16" t="n">
-        <v>3450000</v>
+        <v>1623404</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>1348532</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1464434</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>1870000</v>
+      </c>
+      <c r="M16" t="n">
+        <v>9.25722838994451</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Gerente Compras</t>
+          <t>Responsable Liquidacion</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1863500</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>2200000</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>2614457</v>
       </c>
       <c r="F17" t="n">
-        <v>501945.6911764706</v>
+        <v>2362442.666666667</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>2150000</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>2456052</v>
       </c>
       <c r="I17" t="n">
-        <v>2325000</v>
+        <v>2956250</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1741602</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>2002305</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="inlineStr"/>
+        <v>2270000</v>
+      </c>
+      <c r="M17" t="n">
+        <v>22.66123292904927</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Supervisor Depositos</t>
+          <t>Analista Logistica</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1300000</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1600000</v>
       </c>
       <c r="E18" t="n">
-        <v>351875</v>
+        <v>1900000</v>
       </c>
       <c r="F18" t="n">
-        <v>571177.2352941176</v>
+        <v>1762187.285714286</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1250000</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1573400</v>
       </c>
       <c r="I18" t="n">
-        <v>1937270.75</v>
+        <v>1838553.5</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>1407687.5</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>1680392</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="inlineStr"/>
+        <v>1875000</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-6.367085775223877</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Analista Logistica</t>
+          <t>Jefe Ventas</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2519750</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>3225022.5</v>
       </c>
       <c r="E19" t="n">
-        <v>1225000</v>
+        <v>4300050</v>
       </c>
       <c r="F19" t="n">
-        <v>544204.8970588235</v>
+        <v>3578490.85</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>2910024</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>4200000</v>
       </c>
       <c r="I19" t="n">
-        <v>1275000</v>
+        <v>4800000</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>2336126.5</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>2684000</v>
       </c>
       <c r="L19" t="n">
-        <v>1003796.75</v>
-      </c>
-      <c r="M19" t="inlineStr"/>
+        <v>3662735</v>
+      </c>
+      <c r="M19" t="n">
+        <v>56.48286140089419</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1259,80 +1283,84 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>2296597.5</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>2840897.5</v>
       </c>
       <c r="E20" t="n">
-        <v>2132500</v>
+        <v>3320583.5</v>
       </c>
       <c r="F20" t="n">
-        <v>902099.8382352941</v>
+        <v>3067139.45</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>2243195</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>2500000</v>
       </c>
       <c r="I20" t="n">
-        <v>2264792.5</v>
+        <v>3121675.5</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>2500000</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>2866795</v>
       </c>
       <c r="L20" t="n">
-        <v>1474108.5</v>
-      </c>
-      <c r="M20" t="inlineStr"/>
+        <v>3552281</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-12.79460163701974</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jefe Planificacion</t>
+          <t>Gerente Rrhh</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>3350311.5</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>4823000</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>6887500</v>
       </c>
       <c r="F21" t="n">
-        <v>640254.7647058824</v>
+        <v>5234530.1</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>4300126</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>6450324</v>
       </c>
       <c r="I21" t="n">
-        <v>2614681.75</v>
+        <v>7700000</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>3127500</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>4061100</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="inlineStr"/>
+        <v>6019573.5</v>
+      </c>
+      <c r="M21" t="n">
+        <v>58.83194208465687</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1373,271 +1401,271 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>salario_ingeniero_agronomo</t>
+          <t>salario_jefe_admin_conta</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ingeniero Agronomo</t>
+          <t>Jefe Admin Conta</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>salario_director_comercial</t>
+          <t>salario_analista_contabilidad</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Director Comercial</t>
+          <t>Analista Contabilidad</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>salario_gerente_seguridad</t>
+          <t>salario_empleado_administrativo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Gerente Seguridad</t>
+          <t>Empleado Administrativo</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>salario_responsable_sustentabilidad</t>
+          <t>salario_analista_cuentas_pagar</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Responsable Sustentabilidad</t>
+          <t>Analista Cuentas Pagar</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>68</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>salario_diseñador_grafico</t>
+          <t>salario_jefe_produccion</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Diseñador Grafico</t>
+          <t>Jefe Produccion</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>salario_tecnico_calidad</t>
+          <t>salario_ejecutivo_ventas</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tecnico Calidad</t>
+          <t>Ejecutivo Ventas</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>salario_analista_calidad</t>
+          <t>salario_comprador_analista</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Analista Calidad</t>
+          <t>Comprador Analista</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>salario_jefe_calidad</t>
+          <t>salario_gerente_admin_conta</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jefe Calidad</t>
+          <t>Gerente Admin Conta</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>salario_gerente_calidad</t>
+          <t>salario_analista_facturacion</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gerente Calidad</t>
+          <t>Analista Facturacion</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>salario_tecnico_mantenimiento</t>
+          <t>salario_ceo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tecnico Mantenimiento</t>
+          <t>Ceo</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>salario_supervisor_mantenimiento</t>
+          <t>salario_jefe_rrhh</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Supervisor Mantenimiento</t>
+          <t>Jefe Rrhh</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>68</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>salario_jefe_mantenimiento</t>
+          <t>salario_gerente_planta</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jefe Mantenimiento</t>
+          <t>Gerente Planta</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>salario_gerente_mantenimiento</t>
+          <t>salario_analista_admin_personal</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gerente Mantenimiento</t>
+          <t>Analista Admin Personal</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>salario_comprador_analista</t>
+          <t>salario_jefe_compras</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Comprador Analista</t>
+          <t>Jefe Compras</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>salario_jefe_compras</t>
+          <t>salario_analista_cobranzas</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jefe Compras</t>
+          <t>Analista Cobranzas</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>68</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>salario_gerente_compras</t>
+          <t>salario_responsable_liquidacion</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gerente Compras</t>
+          <t>Responsable Liquidacion</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>salario_supervisor_depositos</t>
+          <t>salario_analista_logistica</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Supervisor Depositos</t>
+          <t>Analista Logistica</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>salario_analista_logistica</t>
+          <t>salario_jefe_ventas</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Analista Logistica</t>
+          <t>Jefe Ventas</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -1652,172 +1680,172 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>salario_jefe_planificacion</t>
+          <t>salario_gerente_rrhh</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jefe Planificacion</t>
+          <t>Gerente Rrhh</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>salario_gerente_supply_chain</t>
+          <t>salario_jefe_calidad</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Gerente Supply Chain</t>
+          <t>Jefe Calidad</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>salario_analista_laboratorio</t>
+          <t>salario_analista_control_gestion</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Analista Laboratorio</t>
+          <t>Analista Control Gestion</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>salario_jefe_laboratorio</t>
+          <t>salario_supervisor_produccion</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jefe Laboratorio</t>
+          <t>Supervisor Produccion</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>salario_jefe_seguridad</t>
+          <t>salario_tecnico_mantenimiento</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Jefe Seguridad</t>
+          <t>Tecnico Mantenimiento</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>salario_tecnico_seguridad</t>
+          <t>salario_supervisor_depositos</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Tecnico Seguridad</t>
+          <t>Supervisor Depositos</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>salario_jefe_ingenieria</t>
+          <t>salario_analista_marketing</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jefe Ingenieria</t>
+          <t>Analista Marketing</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>salario_analista_capacitacion</t>
+          <t>salario_asistente_comex</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Analista Capacitacion</t>
+          <t>Asistente Comex</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>salario_joven_profesional</t>
+          <t>salario_jefe_finanzas</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Joven Profesional</t>
+          <t>Jefe Finanzas</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>salario_analista_helpdesk</t>
+          <t>salario_jefe_mantenimiento</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Analista Helpdesk</t>
+          <t>Jefe Mantenimiento</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>68</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>salario_jefe_soporte</t>
+          <t>salario_supervisor_mantenimiento</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Jefe Soporte</t>
+          <t>Supervisor Mantenimiento</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>68</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>